<commit_message>
Revised import for new format
</commit_message>
<xml_diff>
--- a/app-server/src/main/resources/2021_tracks.xlsx
+++ b/app-server/src/main/resources/2021_tracks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/code/acmsac/app-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC3CDA7-EDDE-394C-A366-0D157D0B4B68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2A2703-DA25-CF4D-B8BB-DD1A338F4BE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="460" windowWidth="27240" windowHeight="16440" xr2:uid="{C929C32E-19ED-9548-9520-722DBCE69E7D}"/>
+    <workbookView xWindow="7660" yWindow="460" windowWidth="27240" windowHeight="16440" xr2:uid="{C929C32E-19ED-9548-9520-722DBCE69E7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23ECFF82-E805-4B4A-B1F7-D4BE15B4EB25}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>